<commit_message>
update: draw cost, GHG, BIO
</commit_message>
<xml_diff>
--- a/myCode/carbonprice/code/tools/land use colors.xlsx
+++ b/myCode/carbonprice/code/tools/land use colors.xlsx
@@ -1,28 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\LUF-Modelling\LUTO2_XH\LUTO2\myCode\draw_all\code\tools\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\school-les-m.shares.deakin.edu.au\school-les-m\Planet-A\LUF-Modelling\LUTO2_XH\LUTO2\myCode\carbonprice\code\tools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A46CE48-30AA-4CF0-8E48-FBB23A6B2F32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18999CAA-AA3E-40A8-98A0-327A13DC6485}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="20085" activeTab="2" xr2:uid="{2D26B5C8-6622-43CF-A59E-89E039B01728}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="5" xr2:uid="{2D26B5C8-6622-43CF-A59E-89E039B01728}"/>
   </bookViews>
   <sheets>
     <sheet name="ag" sheetId="1" r:id="rId1"/>
-    <sheet name="ag_group" sheetId="5" r:id="rId2"/>
-    <sheet name="ag_group_map" sheetId="6" r:id="rId3"/>
-    <sheet name="non_ag" sheetId="2" r:id="rId4"/>
-    <sheet name="am" sheetId="3" r:id="rId5"/>
-    <sheet name="lu" sheetId="4" r:id="rId6"/>
-    <sheet name="WS" sheetId="10" r:id="rId7"/>
-    <sheet name="biodiversity" sheetId="9" r:id="rId8"/>
-    <sheet name="food" sheetId="7" r:id="rId9"/>
-    <sheet name="water" sheetId="8" r:id="rId10"/>
+    <sheet name="cost_revenue" sheetId="11" r:id="rId2"/>
+    <sheet name="cost" sheetId="12" r:id="rId3"/>
+    <sheet name="ag_group" sheetId="5" r:id="rId4"/>
+    <sheet name="ag_group_map" sheetId="6" r:id="rId5"/>
+    <sheet name="non_ag" sheetId="2" r:id="rId6"/>
+    <sheet name="am" sheetId="3" r:id="rId7"/>
+    <sheet name="lu" sheetId="4" r:id="rId8"/>
+    <sheet name="WS" sheetId="10" r:id="rId9"/>
+    <sheet name="biodiversity" sheetId="9" r:id="rId10"/>
+    <sheet name="food" sheetId="7" r:id="rId11"/>
+    <sheet name="water" sheetId="8" r:id="rId12"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -34,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="206">
   <si>
     <t>code</t>
   </si>
@@ -150,9 +152,6 @@
     <t>#C8C8C8</t>
   </si>
   <si>
-    <t>BECCS</t>
-  </si>
-  <si>
     <t>Agricultural land-use</t>
   </si>
   <si>
@@ -192,9 +191,6 @@
     <t>#e69800</t>
   </si>
   <si>
-    <t>Ecological grazing</t>
-  </si>
-  <si>
     <t>Savanna burning</t>
   </si>
   <si>
@@ -207,9 +203,6 @@
     <t>Other land-use</t>
   </si>
   <si>
-    <t>#FFFF00</t>
-  </si>
-  <si>
     <t>Transition</t>
   </si>
   <si>
@@ -495,9 +488,6 @@
     <t>Agricultural technology (fertiliser)</t>
   </si>
   <si>
-    <t>Regenerative agriculture (livestock)</t>
-  </si>
-  <si>
     <t>Early dry-season savanna burning</t>
   </si>
   <si>
@@ -520,9 +510,6 @@
   </si>
   <si>
     <t>Farm forestry (hardwood timber + beef)</t>
-  </si>
-  <si>
-    <t>BECCS (Bioenergy with carbon capture and storage)</t>
   </si>
   <si>
     <t>#00a9ee</t>
@@ -571,9 +558,6 @@
     <t>#20B2AA</t>
   </si>
   <si>
-    <t>#FEC7C7</t>
-  </si>
-  <si>
     <t>#A14189</t>
   </si>
   <si>
@@ -590,6 +574,101 @@
   </si>
   <si>
     <t>#298888</t>
+  </si>
+  <si>
+    <t>Ag cost</t>
+  </si>
+  <si>
+    <t>Agmgt cost</t>
+  </si>
+  <si>
+    <t>#cd4975</t>
+  </si>
+  <si>
+    <t>Non-ag cost</t>
+  </si>
+  <si>
+    <t>#9f0e9e</t>
+  </si>
+  <si>
+    <t>Transition(ag→ag)</t>
+  </si>
+  <si>
+    <t>#6200ac</t>
+  </si>
+  <si>
+    <t>#2d688f</t>
+  </si>
+  <si>
+    <t>Ag revenue</t>
+  </si>
+  <si>
+    <t>#19928e</t>
+  </si>
+  <si>
+    <t>Agmgt revenue</t>
+  </si>
+  <si>
+    <t>#35b876</t>
+  </si>
+  <si>
+    <t>Non-ag revenue</t>
+  </si>
+  <si>
+    <t>Transition(ag→ag) cost</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Transition(ag→non-ag) amortised cost</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>#fab431</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>#ec7951</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>desc</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Ag</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Agmgt</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Non-ag</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>#9D1D1D</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>#7575EB</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>#D89CCD</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>#F2A930</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>#8CB266</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Transition(ag→non-ag) amortised</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -600,19 +679,19 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Aptos Narrow"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="8"/>
-      <name val="Aptos Narrow"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="Aptos Narrow"/>
+      <name val="等线"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -978,15 +1057,15 @@
   <dimension ref="A1:C31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="B2" sqref="B2:C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="29.42578125" customWidth="1"/>
+    <col min="2" max="2" width="29.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -997,29 +1076,29 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>-2</v>
       </c>
       <c r="B2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C2" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>-1</v>
       </c>
       <c r="B3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C3" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>0</v>
       </c>
@@ -1027,10 +1106,10 @@
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>1</v>
       </c>
@@ -1038,10 +1117,10 @@
         <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>2</v>
       </c>
@@ -1049,10 +1128,10 @@
         <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>3</v>
       </c>
@@ -1060,10 +1139,10 @@
         <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>4</v>
       </c>
@@ -1071,10 +1150,10 @@
         <v>7</v>
       </c>
       <c r="C8" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>5</v>
       </c>
@@ -1082,10 +1161,10 @@
         <v>8</v>
       </c>
       <c r="C9" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>6</v>
       </c>
@@ -1093,10 +1172,10 @@
         <v>9</v>
       </c>
       <c r="C10" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>7</v>
       </c>
@@ -1104,10 +1183,10 @@
         <v>10</v>
       </c>
       <c r="C11" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>8</v>
       </c>
@@ -1115,10 +1194,10 @@
         <v>11</v>
       </c>
       <c r="C12" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>9</v>
       </c>
@@ -1126,10 +1205,10 @@
         <v>12</v>
       </c>
       <c r="C13" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>10</v>
       </c>
@@ -1137,10 +1216,10 @@
         <v>13</v>
       </c>
       <c r="C14" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>11</v>
       </c>
@@ -1148,10 +1227,10 @@
         <v>14</v>
       </c>
       <c r="C15" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>12</v>
       </c>
@@ -1159,10 +1238,10 @@
         <v>15</v>
       </c>
       <c r="C16" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>13</v>
       </c>
@@ -1170,10 +1249,10 @@
         <v>16</v>
       </c>
       <c r="C17" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>14</v>
       </c>
@@ -1181,10 +1260,10 @@
         <v>17</v>
       </c>
       <c r="C18" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>15</v>
       </c>
@@ -1192,10 +1271,10 @@
         <v>18</v>
       </c>
       <c r="C19" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>16</v>
       </c>
@@ -1203,10 +1282,10 @@
         <v>19</v>
       </c>
       <c r="C20" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>17</v>
       </c>
@@ -1214,10 +1293,10 @@
         <v>20</v>
       </c>
       <c r="C21" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>18</v>
       </c>
@@ -1225,10 +1304,10 @@
         <v>21</v>
       </c>
       <c r="C22" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>19</v>
       </c>
@@ -1236,10 +1315,10 @@
         <v>22</v>
       </c>
       <c r="C23" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>20</v>
       </c>
@@ -1247,10 +1326,10 @@
         <v>23</v>
       </c>
       <c r="C24" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>21</v>
       </c>
@@ -1258,10 +1337,10 @@
         <v>24</v>
       </c>
       <c r="C25" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>22</v>
       </c>
@@ -1269,10 +1348,10 @@
         <v>31</v>
       </c>
       <c r="C26" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>23</v>
       </c>
@@ -1280,10 +1359,10 @@
         <v>32</v>
       </c>
       <c r="C27" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>24</v>
       </c>
@@ -1291,10 +1370,10 @@
         <v>25</v>
       </c>
       <c r="C28" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>25</v>
       </c>
@@ -1302,10 +1381,10 @@
         <v>26</v>
       </c>
       <c r="C29" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>26</v>
       </c>
@@ -1313,10 +1392,10 @@
         <v>27</v>
       </c>
       <c r="C30" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>27</v>
       </c>
@@ -1324,7 +1403,7 @@
         <v>28</v>
       </c>
       <c r="C31" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
   </sheetData>
@@ -1334,6 +1413,297 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9CB31155-5D49-45D7-B984-2C3E595B567C}">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>142</v>
+      </c>
+      <c r="B2" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="1">
+        <v>0</v>
+      </c>
+      <c r="B3" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="1">
+        <v>0.3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="B5" t="s">
+        <v>145</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1150A691-DE1D-456C-B1D8-8D8F96E1B7AE}">
+  <dimension ref="A1:B27"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="16.125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>90</v>
+      </c>
+      <c r="B3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>91</v>
+      </c>
+      <c r="B4" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>92</v>
+      </c>
+      <c r="B7" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>93</v>
+      </c>
+      <c r="B11" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>94</v>
+      </c>
+      <c r="B13" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>95</v>
+      </c>
+      <c r="B15" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>96</v>
+      </c>
+      <c r="B16" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>97</v>
+      </c>
+      <c r="B17" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>98</v>
+      </c>
+      <c r="B18" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>20</v>
+      </c>
+      <c r="B19" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>99</v>
+      </c>
+      <c r="B20" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>100</v>
+      </c>
+      <c r="B21" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>101</v>
+      </c>
+      <c r="B22" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>102</v>
+      </c>
+      <c r="B23" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>25</v>
+      </c>
+      <c r="B24" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>103</v>
+      </c>
+      <c r="B25" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>104</v>
+      </c>
+      <c r="B26" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>105</v>
+      </c>
+      <c r="B27" t="s">
+        <v>108</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7FE7CEB-5A38-4639-9585-CECD474B9183}">
   <dimension ref="A1:B14"/>
   <sheetViews>
@@ -1341,9 +1711,9 @@
       <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -1351,108 +1721,108 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>109</v>
+      </c>
+      <c r="B2" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>111</v>
+      </c>
+      <c r="B3" t="s">
         <v>112</v>
       </c>
-      <c r="B2" t="s">
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="B4" t="s">
         <v>114</v>
       </c>
-      <c r="B3" t="s">
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="B5" t="s">
         <v>116</v>
       </c>
-      <c r="B4" t="s">
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="B6" t="s">
         <v>118</v>
       </c>
-      <c r="B5" t="s">
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="B7" t="s">
         <v>120</v>
       </c>
-      <c r="B6" t="s">
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="B8" t="s">
         <v>122</v>
       </c>
-      <c r="B7" t="s">
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="B9" t="s">
         <v>124</v>
       </c>
-      <c r="B8" t="s">
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="B10" t="s">
         <v>126</v>
       </c>
-      <c r="B9" t="s">
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="B11" t="s">
         <v>128</v>
       </c>
-      <c r="B10" t="s">
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="B12" t="s">
         <v>130</v>
       </c>
-      <c r="B11" t="s">
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="B13" t="s">
         <v>132</v>
       </c>
-      <c r="B12" t="s">
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="B14" t="s">
         <v>134</v>
-      </c>
-      <c r="B13" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>136</v>
-      </c>
-      <c r="B14" t="s">
-        <v>137</v>
       </c>
     </row>
   </sheetData>
@@ -1462,6 +1832,161 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2E1A99C-7B94-4857-9266-930B7A9F826A}">
+  <dimension ref="A1:B9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="21.125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>179</v>
+      </c>
+      <c r="B2" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>180</v>
+      </c>
+      <c r="B3" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>182</v>
+      </c>
+      <c r="B4" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>192</v>
+      </c>
+      <c r="B5" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>193</v>
+      </c>
+      <c r="B6" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>187</v>
+      </c>
+      <c r="B7" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>189</v>
+      </c>
+      <c r="B8" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>191</v>
+      </c>
+      <c r="B9" t="s">
+        <v>190</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79FA374C-0E4D-4749-A069-80B352085307}">
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>196</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>197</v>
+      </c>
+      <c r="B2" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>198</v>
+      </c>
+      <c r="B3" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>199</v>
+      </c>
+      <c r="B4" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>184</v>
+      </c>
+      <c r="B5" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>205</v>
+      </c>
+      <c r="B6" t="s">
+        <v>204</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{542D8A7D-3A34-4AE5-8DF9-937CC1CA2F8F}">
   <dimension ref="A1:B6"/>
   <sheetViews>
@@ -1469,12 +1994,12 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="34.28515625" customWidth="1"/>
+    <col min="1" max="1" width="34.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -1482,7 +2007,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>29</v>
       </c>
@@ -1490,7 +2015,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>30</v>
       </c>
@@ -1498,15 +2023,15 @@
         <v>35</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>31</v>
       </c>
       <c r="B4" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>32</v>
       </c>
@@ -1514,12 +2039,12 @@
         <v>36</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>33</v>
       </c>
       <c r="B6" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
   </sheetData>
@@ -1528,20 +2053,20 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03998123-DD7C-419B-B0BE-8EDD79757136}">
   <dimension ref="A1:C31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="27.28515625" customWidth="1"/>
+    <col min="2" max="2" width="27.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1552,29 +2077,29 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>-2</v>
       </c>
       <c r="B2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C2" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>-1</v>
       </c>
       <c r="B3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C3" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>0</v>
       </c>
@@ -1585,7 +2110,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>1</v>
       </c>
@@ -1596,7 +2121,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>2</v>
       </c>
@@ -1607,7 +2132,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>3</v>
       </c>
@@ -1618,7 +2143,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>4</v>
       </c>
@@ -1629,7 +2154,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>5</v>
       </c>
@@ -1640,7 +2165,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>6</v>
       </c>
@@ -1651,7 +2176,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>7</v>
       </c>
@@ -1662,7 +2187,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>8</v>
       </c>
@@ -1673,7 +2198,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>9</v>
       </c>
@@ -1684,7 +2209,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>10</v>
       </c>
@@ -1695,7 +2220,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>11</v>
       </c>
@@ -1706,7 +2231,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>12</v>
       </c>
@@ -1717,7 +2242,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>13</v>
       </c>
@@ -1728,7 +2253,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>14</v>
       </c>
@@ -1739,7 +2264,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>15</v>
       </c>
@@ -1750,7 +2275,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>16</v>
       </c>
@@ -1761,7 +2286,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>17</v>
       </c>
@@ -1772,7 +2297,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>18</v>
       </c>
@@ -1783,7 +2308,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>19</v>
       </c>
@@ -1794,7 +2319,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>20</v>
       </c>
@@ -1805,7 +2330,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>21</v>
       </c>
@@ -1816,7 +2341,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>22</v>
       </c>
@@ -1824,10 +2349,10 @@
         <v>31</v>
       </c>
       <c r="C26" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>23</v>
       </c>
@@ -1838,7 +2363,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>24</v>
       </c>
@@ -1849,7 +2374,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>25</v>
       </c>
@@ -1860,7 +2385,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>26</v>
       </c>
@@ -1871,7 +2396,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>27</v>
       </c>
@@ -1888,20 +2413,20 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{271481C8-FF0A-48F8-A9EA-651D41279C7C}">
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="26.28515625" customWidth="1"/>
+    <col min="2" max="2" width="26.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1912,161 +2437,147 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2">
-        <v>100</v>
+        <v>108</v>
       </c>
       <c r="B2" t="s">
-        <v>60</v>
+        <v>168</v>
       </c>
       <c r="C2" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="D2" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="B3" t="s">
         <v>61</v>
       </c>
       <c r="C3" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="D3" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B4" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C4" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D4" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="B5" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="C5" t="s">
         <v>46</v>
       </c>
       <c r="D5" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B6" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="C6" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="D6" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7">
+        <v>103</v>
+      </c>
+      <c r="B7" t="s">
+        <v>60</v>
+      </c>
+      <c r="C7" t="s">
+        <v>45</v>
+      </c>
+      <c r="D7" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8">
         <v>105</v>
       </c>
-      <c r="B7" t="s">
-        <v>65</v>
-      </c>
-      <c r="C7" t="s">
-        <v>177</v>
-      </c>
-      <c r="D7" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8">
+      <c r="B8" t="s">
+        <v>62</v>
+      </c>
+      <c r="C8" t="s">
+        <v>172</v>
+      </c>
+      <c r="D8" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9">
         <v>106</v>
       </c>
-      <c r="B8" t="s">
-        <v>66</v>
-      </c>
-      <c r="C8" t="s">
-        <v>174</v>
-      </c>
-      <c r="D8" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>107</v>
-      </c>
       <c r="B9" t="s">
+        <v>63</v>
+      </c>
+      <c r="C9" t="s">
+        <v>169</v>
+      </c>
+      <c r="D9" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>0</v>
+      </c>
+      <c r="B10" t="s">
         <v>38</v>
       </c>
-      <c r="C9" t="s">
-        <v>57</v>
-      </c>
-      <c r="D9" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>108</v>
-      </c>
-      <c r="B10" t="s">
-        <v>173</v>
-      </c>
       <c r="C10" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="D10" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="B11" t="s">
-        <v>39</v>
+        <v>54</v>
       </c>
       <c r="C11" t="s">
-        <v>37</v>
+        <v>135</v>
       </c>
       <c r="D11" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>-1</v>
-      </c>
-      <c r="B12" t="s">
-        <v>56</v>
-      </c>
-      <c r="C12" t="s">
-        <v>138</v>
-      </c>
-      <c r="D12" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -2076,20 +2587,20 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A38EA70F-F7E1-4FC1-B8F0-19903766E439}">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="L34" sqref="L34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="14.140625" customWidth="1"/>
+    <col min="2" max="2" width="14.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2100,147 +2611,133 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>137</v>
+      </c>
+      <c r="C2" t="s">
+        <v>138</v>
+      </c>
+      <c r="D2" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C3" t="s">
+        <v>158</v>
+      </c>
+      <c r="D3" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C4" t="s">
+        <v>173</v>
+      </c>
+      <c r="D4" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>2</v>
+      </c>
+      <c r="B5" t="s">
         <v>49</v>
       </c>
-      <c r="C2" t="s">
-        <v>163</v>
-      </c>
-      <c r="D2" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
+      <c r="C5" t="s">
         <v>50</v>
       </c>
-      <c r="C3" t="s">
-        <v>51</v>
-      </c>
-      <c r="D3" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>52</v>
-      </c>
-      <c r="C4" t="s">
-        <v>178</v>
-      </c>
-      <c r="D4" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>53</v>
-      </c>
-      <c r="C5" t="s">
-        <v>179</v>
-      </c>
       <c r="D5" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
+        <v>52</v>
+      </c>
+      <c r="C6" t="s">
+        <v>53</v>
+      </c>
+      <c r="D6" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>7</v>
+      </c>
+      <c r="B7" t="s">
+        <v>170</v>
+      </c>
+      <c r="C7" t="s">
+        <v>178</v>
+      </c>
+      <c r="D7" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>8</v>
+      </c>
+      <c r="B8" t="s">
+        <v>171</v>
+      </c>
+      <c r="C8" t="s">
+        <v>177</v>
+      </c>
+      <c r="D8" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>0</v>
+      </c>
+      <c r="B9" t="s">
+        <v>136</v>
+      </c>
+      <c r="C9" t="s">
+        <v>37</v>
+      </c>
+      <c r="D9" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>-1</v>
+      </c>
+      <c r="B10" t="s">
         <v>54</v>
       </c>
-      <c r="C6" t="s">
-        <v>55</v>
-      </c>
-      <c r="D6" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
-        <v>140</v>
-      </c>
-      <c r="C7" t="s">
-        <v>141</v>
-      </c>
-      <c r="D7" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>7</v>
-      </c>
-      <c r="B8" t="s">
-        <v>175</v>
-      </c>
-      <c r="C8" t="s">
-        <v>184</v>
-      </c>
-      <c r="D8" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>8</v>
-      </c>
-      <c r="B9" t="s">
-        <v>176</v>
-      </c>
-      <c r="C9" t="s">
-        <v>183</v>
-      </c>
-      <c r="D9" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>0</v>
-      </c>
-      <c r="B10" t="s">
-        <v>139</v>
-      </c>
       <c r="C10" t="s">
-        <v>37</v>
+        <v>135</v>
       </c>
       <c r="D10" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>-1</v>
-      </c>
-      <c r="B11" t="s">
-        <v>56</v>
-      </c>
-      <c r="C11" t="s">
-        <v>138</v>
-      </c>
-      <c r="D11" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -2249,7 +2746,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{043FD979-195F-4385-BB3B-446A90186897}">
   <dimension ref="A1:B7"/>
   <sheetViews>
@@ -2257,12 +2754,12 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="28.42578125" customWidth="1"/>
+    <col min="1" max="1" width="28.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -2270,52 +2767,52 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B2" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B3" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>39</v>
       </c>
-      <c r="B2" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="B4" t="s">
         <v>41</v>
       </c>
-      <c r="B3" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>40</v>
-      </c>
-      <c r="B4" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="B5" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="B6" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="B7" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
     </row>
   </sheetData>
@@ -2324,7 +2821,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC61CAFA-DABC-40F0-B6E6-C2D5A426B2B8}">
   <dimension ref="A1:B3"/>
   <sheetViews>
@@ -2332,9 +2829,9 @@
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -2342,311 +2839,20 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="B2" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="B3" t="s">
-        <v>168</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9CB31155-5D49-45D7-B984-2C3E595B567C}">
-  <dimension ref="A1:B5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>145</v>
-      </c>
-      <c r="B2" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
-        <v>0</v>
-      </c>
-      <c r="B3" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
-        <v>0.3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
-        <v>0.5</v>
-      </c>
-      <c r="B5" t="s">
-        <v>148</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1150A691-DE1D-456C-B1D8-8D8F96E1B7AE}">
-  <dimension ref="A1:B27"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="16.140625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>93</v>
-      </c>
-      <c r="B3" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>94</v>
-      </c>
-      <c r="B4" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>95</v>
-      </c>
-      <c r="B7" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>10</v>
-      </c>
-      <c r="B8" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>11</v>
-      </c>
-      <c r="B9" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>12</v>
-      </c>
-      <c r="B10" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>96</v>
-      </c>
-      <c r="B11" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>14</v>
-      </c>
-      <c r="B12" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>97</v>
-      </c>
-      <c r="B13" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>16</v>
-      </c>
-      <c r="B14" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>98</v>
-      </c>
-      <c r="B15" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>99</v>
-      </c>
-      <c r="B16" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>100</v>
-      </c>
-      <c r="B17" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>101</v>
-      </c>
-      <c r="B18" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>20</v>
-      </c>
-      <c r="B19" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>102</v>
-      </c>
-      <c r="B20" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>103</v>
-      </c>
-      <c r="B21" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>104</v>
-      </c>
-      <c r="B22" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>105</v>
-      </c>
-      <c r="B23" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>25</v>
-      </c>
-      <c r="B24" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>106</v>
-      </c>
-      <c r="B25" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>107</v>
-      </c>
-      <c r="B26" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>108</v>
-      </c>
-      <c r="B27" t="s">
-        <v>111</v>
+        <v>163</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update: output biodiversity with cut off
</commit_message>
<xml_diff>
--- a/myCode/carbonprice/code/tools/land use colors.xlsx
+++ b/myCode/carbonprice/code/tools/land use colors.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\school-les-m.shares.deakin.edu.au\school-les-m\Planet-A\LUF-Modelling\LUTO2_XH\LUTO2\myCode\carbonprice\code\tools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18999CAA-AA3E-40A8-98A0-327A13DC6485}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6D06095-5D0C-4FE3-A876-2070CD5D1A58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="5" xr2:uid="{2D26B5C8-6622-43CF-A59E-89E039B01728}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{2D26B5C8-6622-43CF-A59E-89E039B01728}"/>
   </bookViews>
   <sheets>
     <sheet name="ag" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="206">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="206">
   <si>
     <t>code</t>
   </si>
@@ -647,35 +647,30 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>#9D1D1D</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>#7575EB</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>#D89CCD</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>#F2A930</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>#8CB266</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>Transition(ag→non-ag) amortised</t>
     <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>#f39b8b</t>
+  </si>
+  <si>
+    <t>#9A8AB3</t>
+  </si>
+  <si>
+    <t>#6eabb1</t>
+  </si>
+  <si>
+    <t>#eb9132</t>
+  </si>
+  <si>
+    <t>#84a374</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -691,6 +686,14 @@
     </font>
     <font>
       <sz val="9"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="等线"/>
       <family val="3"/>
       <charset val="134"/>
@@ -717,9 +720,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1836,7 +1840,7 @@
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="A5" sqref="A5:B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1878,18 +1882,18 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="B5" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B6" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
@@ -1924,13 +1928,16 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79FA374C-0E4D-4749-A069-80B352085307}">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="24.875" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -1940,49 +1947,58 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>197</v>
       </c>
-      <c r="B2" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B2" s="2" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>198</v>
       </c>
-      <c r="B3" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B3" s="2" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>199</v>
       </c>
-      <c r="B4" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B4" s="2" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>184</v>
       </c>
-      <c r="B5" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B5" s="2" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>200</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>205</v>
       </c>
-      <c r="B6" t="s">
+    </row>
+    <row r="7" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>55</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>204</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2417,7 +2433,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{271481C8-FF0A-48F8-A9EA-651D41279C7C}">
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
@@ -2751,7 +2767,7 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
update: output for draw map
</commit_message>
<xml_diff>
--- a/myCode/carbonprice/code/tools/land use colors.xlsx
+++ b/myCode/carbonprice/code/tools/land use colors.xlsx
@@ -8,23 +8,25 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\school-les-m.shares.deakin.edu.au\school-les-m\Planet-A\LUF-Modelling\LUTO2_XH\LUTO2\myCode\carbonprice\code\tools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6D06095-5D0C-4FE3-A876-2070CD5D1A58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A49728C-5A94-49B8-89E1-371855580FD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{2D26B5C8-6622-43CF-A59E-89E039B01728}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="8" xr2:uid="{2D26B5C8-6622-43CF-A59E-89E039B01728}"/>
   </bookViews>
   <sheets>
     <sheet name="ag" sheetId="1" r:id="rId1"/>
     <sheet name="cost_revenue" sheetId="11" r:id="rId2"/>
     <sheet name="cost" sheetId="12" r:id="rId3"/>
-    <sheet name="ag_group" sheetId="5" r:id="rId4"/>
-    <sheet name="ag_group_map" sheetId="6" r:id="rId5"/>
-    <sheet name="non_ag" sheetId="2" r:id="rId6"/>
-    <sheet name="am" sheetId="3" r:id="rId7"/>
-    <sheet name="lu" sheetId="4" r:id="rId8"/>
-    <sheet name="WS" sheetId="10" r:id="rId9"/>
-    <sheet name="biodiversity" sheetId="9" r:id="rId10"/>
-    <sheet name="food" sheetId="7" r:id="rId11"/>
-    <sheet name="water" sheetId="8" r:id="rId12"/>
+    <sheet name="carbon_total" sheetId="13" r:id="rId4"/>
+    <sheet name="biodiversity_total" sheetId="14" r:id="rId5"/>
+    <sheet name="ag_group" sheetId="5" r:id="rId6"/>
+    <sheet name="ag_group_map" sheetId="6" r:id="rId7"/>
+    <sheet name="non_ag" sheetId="2" r:id="rId8"/>
+    <sheet name="am" sheetId="3" r:id="rId9"/>
+    <sheet name="lu" sheetId="4" r:id="rId10"/>
+    <sheet name="WS" sheetId="10" r:id="rId11"/>
+    <sheet name="biodiversity" sheetId="9" r:id="rId12"/>
+    <sheet name="food" sheetId="7" r:id="rId13"/>
+    <sheet name="water" sheetId="8" r:id="rId14"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -36,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="206">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="375" uniqueCount="209">
   <si>
     <t>code</t>
   </si>
@@ -561,12 +563,6 @@
     <t>#A14189</t>
   </si>
   <si>
-    <t>Human-Induced Regeneration (beef)</t>
-  </si>
-  <si>
-    <t>Human-Induced Regeneration (sheep)</t>
-  </si>
-  <si>
     <t>Destocked (natural land)</t>
   </si>
   <si>
@@ -639,10 +635,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>Agmgt</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>Non-ag</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -664,6 +656,30 @@
   </si>
   <si>
     <t>#84a374</t>
+  </si>
+  <si>
+    <t>AgMgt</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Agricultural management</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Agricultural land-use</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Non-agricultural land-use</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Managed regeneration (beef)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Managed regeneration (sheep)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -1417,6 +1433,121 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{043FD979-195F-4385-BB3B-446A90186897}">
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="28.375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B2" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B3" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>55</v>
+      </c>
+      <c r="B5" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>139</v>
+      </c>
+      <c r="B6" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>141</v>
+      </c>
+      <c r="B7" t="s">
+        <v>140</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC61CAFA-DABC-40F0-B6E6-C2D5A426B2B8}">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>161</v>
+      </c>
+      <c r="B2" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>162</v>
+      </c>
+      <c r="B3" t="s">
+        <v>163</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9CB31155-5D49-45D7-B984-2C3E595B567C}">
   <dimension ref="A1:B5"/>
   <sheetViews>
@@ -1472,7 +1603,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1150A691-DE1D-456C-B1D8-8D8F96E1B7AE}">
   <dimension ref="A1:B27"/>
   <sheetViews>
@@ -1707,7 +1838,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7FE7CEB-5A38-4639-9585-CECD474B9183}">
   <dimension ref="A1:B14"/>
   <sheetViews>
@@ -1858,66 +1989,66 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B2" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B3" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B4" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B5" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B6" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B7" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B8" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B9" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
   </sheetData>
@@ -1928,10 +2059,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79FA374C-0E4D-4749-A069-80B352085307}">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1939,60 +2070,70 @@
     <col min="1" max="1" width="24.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C1" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>195</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="C2" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>203</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="C3" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>196</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="C4" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>182</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="C5" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>197</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>198</v>
-      </c>
-      <c r="B3" s="2" t="s">
+      <c r="B6" s="2" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>199</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>184</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>200</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>55</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>204</v>
+      <c r="C6" t="s">
+        <v>197</v>
       </c>
     </row>
   </sheetData>
@@ -2003,6 +2144,140 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{487387C3-A780-4426-9D53-F971330CC4C8}">
+  <dimension ref="A1:C5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="16.375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>194</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>195</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="C2" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>203</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="C3" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>196</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="C4" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>55</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="C5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A15507E-5437-48B6-9ABC-E9D45D30BB8C}">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>194</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>195</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="C2" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>203</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="C3" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>196</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="C4" t="s">
+        <v>206</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{542D8A7D-3A34-4AE5-8DF9-937CC1CA2F8F}">
   <dimension ref="A1:B6"/>
   <sheetViews>
@@ -2069,7 +2344,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03998123-DD7C-419B-B0BE-8EDD79757136}">
   <dimension ref="A1:C31"/>
   <sheetViews>
@@ -2429,12 +2704,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{271481C8-FF0A-48F8-A9EA-651D41279C7C}">
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2467,7 +2742,7 @@
         <v>42</v>
       </c>
       <c r="D2" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -2603,12 +2878,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A38EA70F-F7E1-4FC1-B8F0-19903766E439}">
   <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L34" sqref="L34"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2708,10 +2983,10 @@
         <v>170</v>
       </c>
       <c r="C7" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="D7" t="s">
-        <v>174</v>
+        <v>207</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -2722,10 +2997,10 @@
         <v>171</v>
       </c>
       <c r="C8" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="D8" t="s">
-        <v>175</v>
+        <v>208</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -2754,121 +3029,6 @@
       </c>
       <c r="D10" t="s">
         <v>54</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{043FD979-195F-4385-BB3B-446A90186897}">
-  <dimension ref="A1:B7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="28.375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>38</v>
-      </c>
-      <c r="B2" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>40</v>
-      </c>
-      <c r="B3" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>39</v>
-      </c>
-      <c r="B4" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>55</v>
-      </c>
-      <c r="B5" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>139</v>
-      </c>
-      <c r="B6" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>141</v>
-      </c>
-      <c r="B7" t="s">
-        <v>140</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC61CAFA-DABC-40F0-B6E6-C2D5A426B2B8}">
-  <dimension ref="A1:B3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>161</v>
-      </c>
-      <c r="B2" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>162</v>
-      </c>
-      <c r="B3" t="s">
-        <v>163</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update: create productivity and FLC input data
</commit_message>
<xml_diff>
--- a/myCode/carbonprice/code/tools/land use colors.xlsx
+++ b/myCode/carbonprice/code/tools/land use colors.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\school-les-m.shares.deakin.edu.au\school-les-m\Planet-A\LUF-Modelling\LUTO2_XH\LUTO2\myCode\carbonprice\code\tools\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\LUF-Modelling\LUTO2_XH\LUTO2\myCode\carbonprice\code\tools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9E903A5B-0832-453F-AD90-3D5F181C4507}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96B22E5F-3236-47E2-9003-3672A84D8F22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="6" xr2:uid="{2D26B5C8-6622-43CF-A59E-89E039B01728}"/>
+    <workbookView xWindow="2685" yWindow="2685" windowWidth="23850" windowHeight="12885" xr2:uid="{2D26B5C8-6622-43CF-A59E-89E039B01728}"/>
   </bookViews>
   <sheets>
     <sheet name="ag" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="375" uniqueCount="209">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="366" uniqueCount="200">
   <si>
     <t>code</t>
   </si>
@@ -181,9 +181,6 @@
     <t>#267300</t>
   </si>
   <si>
-    <t>#F2A361</t>
-  </si>
-  <si>
     <t>Asparagopsis taxiformis</t>
   </si>
   <si>
@@ -223,15 +220,6 @@
     <t>Beef agroforestry</t>
   </si>
   <si>
-    <t>Carbon plantings (Block)</t>
-  </si>
-  <si>
-    <t>Sheep carbon plantings (Belt)</t>
-  </si>
-  <si>
-    <t>Beef carbon plantings (Belt)</t>
-  </si>
-  <si>
     <t>#1f77b4</t>
   </si>
   <si>
@@ -503,15 +491,6 @@
   </si>
   <si>
     <t>Agroforestry (mixed species + beef)</t>
-  </si>
-  <si>
-    <t>Carbon plantings (monoculture)</t>
-  </si>
-  <si>
-    <t>Farm forestry (hardwood timber + sheep)</t>
-  </si>
-  <si>
-    <t>Farm forestry (hardwood timber + beef)</t>
   </si>
   <si>
     <t>#00a9ee</t>
@@ -548,16 +527,10 @@
     <t>Destocked - natural land</t>
   </si>
   <si>
-    <t>#A0522D</t>
-  </si>
-  <si>
     <t>HIR - Beef</t>
   </si>
   <si>
     <t>HIR - Sheep</t>
-  </si>
-  <si>
-    <t>#20B2AA</t>
   </si>
   <si>
     <t>#A14189</t>
@@ -686,19 +659,19 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="等线"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="8"/>
-      <name val="等线"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="等线"/>
+      <name val="Aptos Narrow"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -706,7 +679,7 @@
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
-      <name val="等线"/>
+      <name val="Aptos Narrow"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -732,11 +705,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1073,16 +1045,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12AAFD40-B427-44B8-B76D-76BB3E7A0B59}">
   <dimension ref="A1:C31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:C7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="29.375" customWidth="1"/>
+    <col min="2" max="2" width="29.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1093,29 +1065,29 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>-2</v>
       </c>
       <c r="B2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C2" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>-1</v>
       </c>
       <c r="B3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C3" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>0</v>
       </c>
@@ -1123,10 +1095,10 @@
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1</v>
       </c>
@@ -1134,10 +1106,10 @@
         <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2</v>
       </c>
@@ -1145,10 +1117,10 @@
         <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>3</v>
       </c>
@@ -1156,10 +1128,10 @@
         <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>4</v>
       </c>
@@ -1167,10 +1139,10 @@
         <v>7</v>
       </c>
       <c r="C8" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>5</v>
       </c>
@@ -1178,10 +1150,10 @@
         <v>8</v>
       </c>
       <c r="C9" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>6</v>
       </c>
@@ -1189,10 +1161,10 @@
         <v>9</v>
       </c>
       <c r="C10" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>7</v>
       </c>
@@ -1200,10 +1172,10 @@
         <v>10</v>
       </c>
       <c r="C11" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>8</v>
       </c>
@@ -1211,10 +1183,10 @@
         <v>11</v>
       </c>
       <c r="C12" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>9</v>
       </c>
@@ -1222,10 +1194,10 @@
         <v>12</v>
       </c>
       <c r="C13" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>10</v>
       </c>
@@ -1233,10 +1205,10 @@
         <v>13</v>
       </c>
       <c r="C14" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>11</v>
       </c>
@@ -1244,10 +1216,10 @@
         <v>14</v>
       </c>
       <c r="C15" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>12</v>
       </c>
@@ -1255,10 +1227,10 @@
         <v>15</v>
       </c>
       <c r="C16" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>13</v>
       </c>
@@ -1266,10 +1238,10 @@
         <v>16</v>
       </c>
       <c r="C17" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>14</v>
       </c>
@@ -1277,10 +1249,10 @@
         <v>17</v>
       </c>
       <c r="C18" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>15</v>
       </c>
@@ -1288,10 +1260,10 @@
         <v>18</v>
       </c>
       <c r="C19" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>16</v>
       </c>
@@ -1299,10 +1271,10 @@
         <v>19</v>
       </c>
       <c r="C20" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>17</v>
       </c>
@@ -1310,10 +1282,10 @@
         <v>20</v>
       </c>
       <c r="C21" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>18</v>
       </c>
@@ -1321,10 +1293,10 @@
         <v>21</v>
       </c>
       <c r="C22" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>19</v>
       </c>
@@ -1332,10 +1304,10 @@
         <v>22</v>
       </c>
       <c r="C23" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>20</v>
       </c>
@@ -1343,10 +1315,10 @@
         <v>23</v>
       </c>
       <c r="C24" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>21</v>
       </c>
@@ -1354,10 +1326,10 @@
         <v>24</v>
       </c>
       <c r="C25" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>22</v>
       </c>
@@ -1365,10 +1337,10 @@
         <v>31</v>
       </c>
       <c r="C26" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>23</v>
       </c>
@@ -1376,10 +1348,10 @@
         <v>32</v>
       </c>
       <c r="C27" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>24</v>
       </c>
@@ -1387,10 +1359,10 @@
         <v>25</v>
       </c>
       <c r="C28" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>25</v>
       </c>
@@ -1398,10 +1370,10 @@
         <v>26</v>
       </c>
       <c r="C29" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>26</v>
       </c>
@@ -1409,10 +1381,10 @@
         <v>27</v>
       </c>
       <c r="C30" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>27</v>
       </c>
@@ -1420,7 +1392,7 @@
         <v>28</v>
       </c>
       <c r="C31" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
     </row>
   </sheetData>
@@ -1437,12 +1409,12 @@
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28.375" customWidth="1"/>
+    <col min="1" max="1" width="28.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -1450,23 +1422,23 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>38</v>
       </c>
       <c r="B2" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>40</v>
       </c>
       <c r="B3" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>39</v>
       </c>
@@ -1474,28 +1446,28 @@
         <v>41</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>54</v>
+      </c>
+      <c r="B5" t="s">
         <v>55</v>
       </c>
-      <c r="B5" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="B6" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="B7" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
     </row>
   </sheetData>
@@ -1512,9 +1484,9 @@
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -1522,20 +1494,20 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
       <c r="B2" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="B3" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
     </row>
   </sheetData>
@@ -1552,9 +1524,9 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -1562,36 +1534,36 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>138</v>
+      </c>
+      <c r="B2" t="s">
         <v>142</v>
       </c>
-      <c r="B2" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>0.3</v>
       </c>
       <c r="B4" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>0.5</v>
       </c>
       <c r="B5" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
     </row>
   </sheetData>
@@ -1608,12 +1580,12 @@
       <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.125" customWidth="1"/>
+    <col min="1" max="1" width="16.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -1621,212 +1593,212 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="B3" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="B4" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="B7" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>10</v>
       </c>
       <c r="B8" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>11</v>
       </c>
       <c r="B9" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>12</v>
       </c>
       <c r="B10" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="B11" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>14</v>
       </c>
       <c r="B12" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="B13" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>16</v>
       </c>
       <c r="B14" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>91</v>
+      </c>
+      <c r="B15" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>92</v>
+      </c>
+      <c r="B16" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>93</v>
+      </c>
+      <c r="B17" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>94</v>
+      </c>
+      <c r="B18" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>95</v>
-      </c>
-      <c r="B15" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>96</v>
-      </c>
-      <c r="B16" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>97</v>
-      </c>
-      <c r="B17" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>98</v>
-      </c>
-      <c r="B18" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>20</v>
       </c>
       <c r="B19" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>95</v>
+      </c>
+      <c r="B20" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>96</v>
+      </c>
+      <c r="B21" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>97</v>
+      </c>
+      <c r="B22" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>98</v>
+      </c>
+      <c r="B23" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>99</v>
-      </c>
-      <c r="B20" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>100</v>
-      </c>
-      <c r="B21" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>101</v>
-      </c>
-      <c r="B22" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
-        <v>102</v>
-      </c>
-      <c r="B23" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>25</v>
       </c>
       <c r="B24" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
+        <v>99</v>
+      </c>
+      <c r="B25" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>100</v>
+      </c>
+      <c r="B26" t="s">
         <v>103</v>
       </c>
-      <c r="B25" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>101</v>
+      </c>
+      <c r="B27" t="s">
         <v>104</v>
-      </c>
-      <c r="B26" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
-        <v>105</v>
-      </c>
-      <c r="B27" t="s">
-        <v>108</v>
       </c>
     </row>
   </sheetData>
@@ -1843,9 +1815,9 @@
       <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -1853,108 +1825,108 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>105</v>
+      </c>
+      <c r="B2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>107</v>
+      </c>
+      <c r="B3" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>109</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B4" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>111</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B5" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>113</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B6" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>115</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B7" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>117</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B8" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>119</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B9" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>121</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B10" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>123</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B11" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>125</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B12" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>127</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B13" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>129</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B14" t="s">
         <v>130</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>131</v>
-      </c>
-      <c r="B13" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>133</v>
-      </c>
-      <c r="B14" t="s">
-        <v>134</v>
       </c>
     </row>
   </sheetData>
@@ -1971,81 +1943,81 @@
       <selection sqref="A1:B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.125" customWidth="1"/>
+    <col min="1" max="1" width="21.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>168</v>
+      </c>
+      <c r="B2" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>169</v>
+      </c>
+      <c r="B3" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>171</v>
+      </c>
+      <c r="B4" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>198</v>
+      </c>
+      <c r="B5" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>199</v>
+      </c>
+      <c r="B6" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>176</v>
+      </c>
+      <c r="B7" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>178</v>
+      </c>
+      <c r="B8" t="s">
         <v>177</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" s="3" t="s">
-        <v>178</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" s="3" t="s">
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>180</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B9" t="s">
         <v>179</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" s="3" t="s">
-        <v>207</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" s="3" t="s">
-        <v>208</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" s="3" t="s">
-        <v>185</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" s="3" t="s">
-        <v>187</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" s="3" t="s">
-        <v>189</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>188</v>
       </c>
     </row>
   </sheetData>
@@ -2062,75 +2034,75 @@
       <selection activeCell="C1" sqref="C1:C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.875" customWidth="1"/>
+    <col min="1" max="1" width="24.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>190</v>
+        <v>181</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>191</v>
+        <v>182</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>194</v>
+        <v>185</v>
       </c>
       <c r="C2" t="s">
-        <v>201</v>
+        <v>192</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>199</v>
+        <v>190</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>195</v>
+        <v>186</v>
       </c>
       <c r="C3" t="s">
-        <v>200</v>
+        <v>191</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>192</v>
+        <v>183</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>196</v>
+        <v>187</v>
       </c>
       <c r="C4" t="s">
-        <v>202</v>
+        <v>193</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>182</v>
+        <v>173</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>197</v>
+        <v>188</v>
       </c>
       <c r="C5" t="s">
-        <v>182</v>
+        <v>173</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>193</v>
+        <v>184</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>198</v>
+        <v>189</v>
       </c>
       <c r="C6" t="s">
-        <v>193</v>
+        <v>184</v>
       </c>
     </row>
   </sheetData>
@@ -2148,64 +2120,64 @@
       <selection activeCell="C1" sqref="C1:C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.375" customWidth="1"/>
+    <col min="1" max="1" width="16.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>190</v>
+        <v>181</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>191</v>
+        <v>182</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>194</v>
+        <v>185</v>
       </c>
       <c r="C2" t="s">
-        <v>201</v>
+        <v>192</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>199</v>
+        <v>190</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>195</v>
+        <v>186</v>
       </c>
       <c r="C3" t="s">
-        <v>200</v>
+        <v>191</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>192</v>
+        <v>183</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>196</v>
+        <v>187</v>
       </c>
       <c r="C4" t="s">
-        <v>202</v>
+        <v>193</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>197</v>
+        <v>188</v>
       </c>
       <c r="C5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -2222,50 +2194,50 @@
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>190</v>
+        <v>181</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>191</v>
+        <v>182</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>194</v>
+        <v>185</v>
       </c>
       <c r="C2" t="s">
-        <v>201</v>
+        <v>192</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>199</v>
+        <v>190</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>195</v>
+        <v>186</v>
       </c>
       <c r="C3" t="s">
-        <v>200</v>
+        <v>191</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>192</v>
+        <v>183</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>196</v>
+        <v>187</v>
       </c>
       <c r="C4" t="s">
-        <v>202</v>
+        <v>193</v>
       </c>
     </row>
   </sheetData>
@@ -2282,12 +2254,12 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="34.25" customWidth="1"/>
+    <col min="1" max="1" width="34.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -2295,7 +2267,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>29</v>
       </c>
@@ -2303,7 +2275,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>30</v>
       </c>
@@ -2311,15 +2283,15 @@
         <v>35</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>31</v>
       </c>
       <c r="B4" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>32</v>
       </c>
@@ -2327,12 +2299,12 @@
         <v>36</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>33</v>
       </c>
       <c r="B6" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
     </row>
   </sheetData>
@@ -2345,16 +2317,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03998123-DD7C-419B-B0BE-8EDD79757136}">
   <dimension ref="A1:C31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="27.25" customWidth="1"/>
+    <col min="2" max="2" width="27.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2365,7 +2337,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>-2</v>
       </c>
@@ -2376,18 +2348,18 @@
         <v>37</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>-1</v>
       </c>
       <c r="B3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C3" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>0</v>
       </c>
@@ -2398,7 +2370,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1</v>
       </c>
@@ -2409,7 +2381,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2</v>
       </c>
@@ -2420,7 +2392,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>3</v>
       </c>
@@ -2431,7 +2403,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>4</v>
       </c>
@@ -2442,7 +2414,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>5</v>
       </c>
@@ -2453,7 +2425,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>6</v>
       </c>
@@ -2464,7 +2436,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>7</v>
       </c>
@@ -2475,7 +2447,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>8</v>
       </c>
@@ -2486,7 +2458,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>9</v>
       </c>
@@ -2497,7 +2469,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>10</v>
       </c>
@@ -2508,7 +2480,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>11</v>
       </c>
@@ -2519,7 +2491,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>12</v>
       </c>
@@ -2530,7 +2502,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>13</v>
       </c>
@@ -2541,7 +2513,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>14</v>
       </c>
@@ -2552,7 +2524,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>15</v>
       </c>
@@ -2563,7 +2535,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>16</v>
       </c>
@@ -2574,7 +2546,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>17</v>
       </c>
@@ -2585,7 +2557,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>18</v>
       </c>
@@ -2596,7 +2568,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>19</v>
       </c>
@@ -2607,7 +2579,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>20</v>
       </c>
@@ -2618,7 +2590,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>21</v>
       </c>
@@ -2629,7 +2601,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>22</v>
       </c>
@@ -2637,10 +2609,10 @@
         <v>31</v>
       </c>
       <c r="C26" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>23</v>
       </c>
@@ -2651,7 +2623,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>24</v>
       </c>
@@ -2662,7 +2634,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>25</v>
       </c>
@@ -2673,7 +2645,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>26</v>
       </c>
@@ -2684,7 +2656,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>27</v>
       </c>
@@ -2703,18 +2675,18 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{271481C8-FF0A-48F8-A9EA-651D41279C7C}">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="26.25" customWidth="1"/>
+    <col min="2" max="2" width="26.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2725,147 +2697,105 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>108</v>
       </c>
       <c r="B2" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="C2" t="s">
         <v>42</v>
       </c>
       <c r="D2" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="B3" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="C3" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="D3" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C4" t="s">
+        <v>46</v>
+      </c>
+      <c r="D4" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>102</v>
+      </c>
+      <c r="B5" t="s">
         <v>58</v>
       </c>
-      <c r="C4" t="s">
-        <v>43</v>
-      </c>
-      <c r="D4" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5">
-        <v>100</v>
-      </c>
-      <c r="B5" t="s">
-        <v>57</v>
-      </c>
       <c r="C5" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D5" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B6" t="s">
         <v>59</v>
       </c>
       <c r="C6" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D6" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>103</v>
+        <v>0</v>
       </c>
       <c r="B7" t="s">
-        <v>60</v>
+        <v>38</v>
       </c>
       <c r="C7" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="D7" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>105</v>
+        <v>-1</v>
       </c>
       <c r="B8" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="C8" t="s">
-        <v>172</v>
+        <v>131</v>
       </c>
       <c r="D8" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9">
-        <v>106</v>
-      </c>
-      <c r="B9" t="s">
-        <v>63</v>
-      </c>
-      <c r="C9" t="s">
-        <v>169</v>
-      </c>
-      <c r="D9" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10">
-        <v>0</v>
-      </c>
-      <c r="B10" t="s">
-        <v>38</v>
-      </c>
-      <c r="C10" t="s">
-        <v>37</v>
-      </c>
-      <c r="D10" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11">
-        <v>-1</v>
-      </c>
-      <c r="B11" t="s">
-        <v>54</v>
-      </c>
-      <c r="C11" t="s">
-        <v>135</v>
-      </c>
-      <c r="D11" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>
@@ -2883,12 +2813,12 @@
       <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="14.125" customWidth="1"/>
+    <col min="2" max="2" width="14.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2899,133 +2829,133 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="C2" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="D2" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C3" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="D3" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C4" t="s">
-        <v>173</v>
+        <v>164</v>
       </c>
       <c r="D4" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2</v>
       </c>
       <c r="B5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C5" t="s">
         <v>49</v>
       </c>
-      <c r="C5" t="s">
-        <v>50</v>
-      </c>
       <c r="D5" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
+        <v>51</v>
+      </c>
+      <c r="C6" t="s">
         <v>52</v>
       </c>
-      <c r="C6" t="s">
-        <v>53</v>
-      </c>
       <c r="D6" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>170</v>
+        <v>162</v>
       </c>
       <c r="C7" t="s">
-        <v>176</v>
+        <v>167</v>
       </c>
       <c r="D7" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>171</v>
+        <v>163</v>
       </c>
       <c r="C8" t="s">
-        <v>175</v>
+        <v>166</v>
       </c>
       <c r="D8" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>0</v>
       </c>
       <c r="B9" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="C9" t="s">
         <v>37</v>
       </c>
       <c r="D9" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>-1</v>
       </c>
       <c r="B10" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C10" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="D10" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>